<commit_message>
add a HowTo in Excel worksheets for localCorr
Signed-off-by: cordHarms <cord.harms@d-fine.de>
</commit_message>
<xml_diff>
--- a/QuantLibXL/Workbooks/Experimental/LocalCorr_StructuredDeals.xlsx
+++ b/QuantLibXL/Workbooks/Experimental/LocalCorr_StructuredDeals.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="144" windowWidth="17220" windowHeight="8616" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="144" windowWidth="17220" windowHeight="8616"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="28" r:id="rId1"/>
@@ -30,12 +30,12 @@
     <definedName name="setting">[2]Sheet1!$A$2:$A$5</definedName>
     <definedName name="spotUL1">[1]EURUSDLocalVol!$G$12</definedName>
   </definedNames>
-  <calcPr calcId="145621" calcMode="manual"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="98">
   <si>
     <t>Key</t>
   </si>
@@ -323,6 +323,12 @@
   </si>
   <si>
     <t>Asset 2 (GBP/USD)</t>
+  </si>
+  <si>
+    <t>/1.01 und 0.99, wegen change of numeraire</t>
+  </si>
+  <si>
+    <t>Caution: This workbook expects a calibrated mcSimulationT object! This object has to be referenced in B2.</t>
   </si>
 </sst>
 </file>
@@ -3730,7 +3736,7 @@
     <xf numFmtId="0" fontId="147" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="146" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
@@ -3998,11 +4004,14 @@
     <xf numFmtId="164" fontId="0" fillId="90" borderId="60" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="90" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="90" borderId="0" xfId="0" quotePrefix="1" applyFill="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="90" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="90" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="819">
@@ -5068,11 +5077,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="170242048"/>
-        <c:axId val="170321408"/>
+        <c:axId val="166854016"/>
+        <c:axId val="167224448"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="170242048"/>
+        <c:axId val="166854016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5082,7 +5091,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="170321408"/>
+        <c:crossAx val="167224448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5090,7 +5099,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="170321408"/>
+        <c:axId val="167224448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5101,7 +5110,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="170242048"/>
+        <c:crossAx val="166854016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5207,16 +5216,16 @@
                 <c:formatCode>0,000</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.43513055139838897</c:v>
+                  <c:v>0.35560764019623714</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.37277714918821714</c:v>
+                  <c:v>0.32804883043442284</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.22328291206461715</c:v>
+                  <c:v>0.20553783904865805</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.3090251557169316E-2</c:v>
+                  <c:v>4.9782703740131377E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5268,16 +5277,16 @@
                 <c:formatCode>0,000</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.41572337075173671</c:v>
+                  <c:v>0.33695231367449824</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.34229577363251229</c:v>
+                  <c:v>0.29816738034818407</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.20155850031494618</c:v>
+                  <c:v>0.18400027071565436</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.5751783233173736E-2</c:v>
+                  <c:v>5.2393537926615115E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5329,16 +5338,16 @@
                 <c:formatCode>0,000</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.43717866975171088</c:v>
+                  <c:v>0.35785674012939261</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.37068004716702058</c:v>
+                  <c:v>0.32599688031770685</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.22584872143995902</c:v>
+                  <c:v>0.20821256785840775</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.0938205219430781E-2</c:v>
+                  <c:v>5.7684103474009082E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5355,11 +5364,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="43152512"/>
-        <c:axId val="43154048"/>
+        <c:axId val="171711104"/>
+        <c:axId val="171712896"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="43152512"/>
+        <c:axId val="171711104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5369,7 +5378,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="43154048"/>
+        <c:crossAx val="171712896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5377,7 +5386,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="43154048"/>
+        <c:axId val="171712896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5388,7 +5397,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="43152512"/>
+        <c:crossAx val="171711104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5757,11 +5766,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="170245504"/>
-        <c:axId val="171119744"/>
+        <c:axId val="171784448"/>
+        <c:axId val="171794432"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="170245504"/>
+        <c:axId val="171784448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.2"/>
@@ -5773,12 +5782,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="171119744"/>
+        <c:crossAx val="171794432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="171119744"/>
+        <c:axId val="171794432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5789,7 +5798,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="170245504"/>
+        <c:crossAx val="171784448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6272,11 +6281,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="124564224"/>
-        <c:axId val="124565760"/>
+        <c:axId val="171818368"/>
+        <c:axId val="171828352"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="124564224"/>
+        <c:axId val="171818368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.2"/>
@@ -6288,12 +6297,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="124565760"/>
+        <c:crossAx val="171828352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="124565760"/>
+        <c:axId val="171828352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6304,7 +6313,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="124564224"/>
+        <c:crossAx val="171818368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6593,6 +6602,70 @@
       <sheetName val="VanillasCross"/>
       <sheetName val="VisualizationLocalCorr"/>
       <sheetName val="Simulation"/>
+      <sheetName val="InterpolatedSurface"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1">
+        <row r="7">
+          <cell r="Q7">
+            <v>0.99353544955456108</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2">
+        <row r="7">
+          <cell r="Q7">
+            <v>0.99062800543374674</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="3">
+        <row r="7">
+          <cell r="Q7">
+            <v>0.9917720444765119</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="4">
+        <row r="4">
+          <cell r="D4" t="str">
+            <v>obj_00397#0012</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="5">
+        <row r="4">
+          <cell r="D4" t="str">
+            <v>obj_003a7#0012</v>
+          </cell>
+        </row>
+        <row r="63">
+          <cell r="D63" t="str">
+            <v>obj_003b8#0013</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="ValuationDate"/>
+      <sheetName val="VolSurface_EURUSD"/>
+      <sheetName val="VolSurface_GBPUSD"/>
+      <sheetName val="VolSurface_EURGBP"/>
+      <sheetName val="Vanillas"/>
+      <sheetName val="VanillasCross"/>
+      <sheetName val="VisualizationLocalCorr"/>
+      <sheetName val="Simulation"/>
       <sheetName val="Sheet1"/>
     </sheetNames>
     <sheetDataSet>
@@ -6676,70 +6749,6 @@
       <sheetData sheetId="6"/>
       <sheetData sheetId="7"/>
       <sheetData sheetId="8"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="ValuationDate"/>
-      <sheetName val="VolSurface_EURUSD"/>
-      <sheetName val="VolSurface_GBPUSD"/>
-      <sheetName val="VolSurface_EURGBP"/>
-      <sheetName val="Vanillas"/>
-      <sheetName val="VanillasCross"/>
-      <sheetName val="VisualizationLocalCorr"/>
-      <sheetName val="Simulation"/>
-      <sheetName val="InterpolatedSurface"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1">
-        <row r="7">
-          <cell r="Q7">
-            <v>0.99353544955456108</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2">
-        <row r="7">
-          <cell r="Q7">
-            <v>0.99062800543374674</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="3">
-        <row r="7">
-          <cell r="Q7">
-            <v>0.9917720444765119</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="4">
-        <row r="4">
-          <cell r="D4" t="str">
-            <v>obj_00397#0012</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="5">
-        <row r="4">
-          <cell r="D4" t="str">
-            <v>obj_003a7#0012</v>
-          </cell>
-        </row>
-        <row r="63">
-          <cell r="D63" t="str">
-            <v>obj_003b8#0013</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -7032,10 +7041,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -7057,8 +7066,13 @@
         <v>77</v>
       </c>
       <c r="B2" t="str">
-        <f>[4]VanillasCross!$D$63</f>
+        <f>[3]VanillasCross!$D$63</f>
         <v>obj_003b8#0013</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -7070,8 +7084,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="P44" sqref="P44"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -7383,12 +7397,12 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="66"/>
-      <c r="B26" s="89" t="s">
+      <c r="B26" s="91" t="s">
         <v>94</v>
       </c>
-      <c r="C26" s="89"/>
-      <c r="D26" s="89"/>
-      <c r="E26" s="89"/>
+      <c r="C26" s="91"/>
+      <c r="D26" s="91"/>
+      <c r="E26" s="91"/>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="66"/>
@@ -7406,7 +7420,7 @@
       </c>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="90" t="s">
+      <c r="A28" s="89" t="s">
         <v>91</v>
       </c>
       <c r="B28" s="88">
@@ -7424,7 +7438,7 @@
       </c>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="90" t="s">
+      <c r="A29" s="89" t="s">
         <v>93</v>
       </c>
       <c r="B29" s="88">
@@ -7441,7 +7455,7 @@
       </c>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="90" t="s">
+      <c r="A30" s="89" t="s">
         <v>92</v>
       </c>
       <c r="B30" s="88">
@@ -7459,14 +7473,14 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="66"/>
-      <c r="B32" s="89" t="s">
+      <c r="B32" s="91" t="s">
         <v>95</v>
       </c>
-      <c r="C32" s="89"/>
-      <c r="D32" s="89"/>
-      <c r="E32" s="89"/>
-    </row>
-    <row r="33" spans="1:5">
+      <c r="C32" s="91"/>
+      <c r="D32" s="91"/>
+      <c r="E32" s="91"/>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33" s="66"/>
       <c r="B33" s="66">
         <v>1.1000000000000001</v>
@@ -7480,57 +7494,60 @@
       <c r="E33" s="66">
         <v>0.95</v>
       </c>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34" s="90" t="s">
+      <c r="F33" s="90" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="89" t="s">
         <v>91</v>
       </c>
       <c r="B34" s="88">
-        <f t="array" ref="B34:E36">TRANSPOSE((D12:F15-A12:C15)/0.02)</f>
-        <v>0.43513055139838897</v>
+        <f t="array" ref="B34:E36">TRANSPOSE((D12:F15/1.01-A12:C15/0.99)/0.02)</f>
+        <v>0.35560764019623714</v>
       </c>
       <c r="C34" s="88">
-        <v>0.37277714918821714</v>
+        <v>0.32804883043442284</v>
       </c>
       <c r="D34" s="88">
-        <v>0.22328291206461715</v>
+        <v>0.20553783904865805</v>
       </c>
       <c r="E34" s="88">
-        <v>5.3090251557169316E-2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35" s="90" t="s">
+        <v>4.9782703740131377E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="89" t="s">
         <v>93</v>
       </c>
       <c r="B35" s="88">
-        <v>0.41572337075173671</v>
+        <v>0.33695231367449824</v>
       </c>
       <c r="C35" s="88">
-        <v>0.34229577363251229</v>
+        <v>0.29816738034818407</v>
       </c>
       <c r="D35" s="88">
-        <v>0.20155850031494618</v>
+        <v>0.18400027071565436</v>
       </c>
       <c r="E35" s="88">
-        <v>5.5751783233173736E-2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36" s="90" t="s">
+        <v>5.2393537926615115E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="89" t="s">
         <v>92</v>
       </c>
       <c r="B36" s="88">
-        <v>0.43717866975171088</v>
+        <v>0.35785674012939261</v>
       </c>
       <c r="C36" s="88">
-        <v>0.37068004716702058</v>
+        <v>0.32599688031770685</v>
       </c>
       <c r="D36" s="88">
-        <v>0.22584872143995902</v>
+        <v>0.20821256785840775</v>
       </c>
       <c r="E36" s="88">
-        <v>6.0938205219430781E-2</v>
+        <v>5.7684103474009082E-2</v>
       </c>
     </row>
   </sheetData>
@@ -8273,19 +8290,19 @@
         <v>4.6269976603527472E-5</v>
       </c>
       <c r="F44" s="71">
-        <f>(F40-$E40)/$E44</f>
+        <f t="shared" ref="F44:I46" si="0">(F40-$E40)/$E44</f>
         <v>1.1206227321070031E-2</v>
       </c>
       <c r="G44" s="71">
-        <f>(G40-$E40)/$E44</f>
+        <f t="shared" si="0"/>
         <v>-1</v>
       </c>
       <c r="H44" s="71">
-        <f>(H40-$E40)/$E44</f>
+        <f t="shared" si="0"/>
         <v>0.81999595937879599</v>
       </c>
       <c r="I44" s="71">
-        <f>(I40-$E40)/$E44</f>
+        <f t="shared" si="0"/>
         <v>-1.4008249132415089</v>
       </c>
       <c r="J44" s="69"/>
@@ -8301,19 +8318,19 @@
         <v>-3.461309200150902E-7</v>
       </c>
       <c r="F45" s="71">
-        <f>(F41-$E41)/$E45</f>
+        <f t="shared" si="0"/>
         <v>-1.1448472844741695</v>
       </c>
       <c r="G45" s="71">
-        <f>(G41-$E41)/$E45</f>
+        <f t="shared" si="0"/>
         <v>-1</v>
       </c>
       <c r="H45" s="71">
-        <f>(H41-$E41)/$E45</f>
+        <f t="shared" si="0"/>
         <v>21.561979248985327</v>
       </c>
       <c r="I45" s="71">
-        <f>(I41-$E41)/$E45</f>
+        <f t="shared" si="0"/>
         <v>-20.1971851461361</v>
       </c>
       <c r="J45" s="69"/>
@@ -8329,19 +8346,19 @@
         <v>1.0909635555701389E-4</v>
       </c>
       <c r="F46" s="71">
-        <f>(F42-$E42)/$E46</f>
+        <f t="shared" si="0"/>
         <v>-2.8215237724606261</v>
       </c>
       <c r="G46" s="71">
-        <f>(G42-$E42)/$E46</f>
+        <f t="shared" si="0"/>
         <v>-1</v>
       </c>
       <c r="H46" s="71">
-        <f>(H42-$E42)/$E46</f>
+        <f t="shared" si="0"/>
         <v>-0.57373651281772542</v>
       </c>
       <c r="I46" s="71">
-        <f>(I42-$E42)/$E46</f>
+        <f t="shared" si="0"/>
         <v>-5.3266610796251452</v>
       </c>
       <c r="J46" s="69"/>
@@ -8365,11 +8382,11 @@
     </row>
     <row r="48" spans="2:13" ht="14.4">
       <c r="C48" s="49">
-        <f>$B$44-D48</f>
+        <f t="shared" ref="C48:C53" si="1">$B$44-D48</f>
         <v>9.69958225160229E-2</v>
       </c>
       <c r="D48" s="48">
-        <f t="array" ref="D48:D58">TRANSPOSE([3]VanillasCross!$P$9:$Z$9)</f>
+        <f t="array" ref="D48:D58">TRANSPOSE([4]VanillasCross!$P$9:$Z$9)</f>
         <v>0.87151206299808792</v>
       </c>
       <c r="E48" s="67">
@@ -8395,7 +8412,7 @@
     </row>
     <row r="49" spans="3:13" ht="14.4">
       <c r="C49" s="49">
-        <f>$B$44-D49</f>
+        <f t="shared" si="1"/>
         <v>6.6345039070730416E-2</v>
       </c>
       <c r="D49" s="48">
@@ -8424,7 +8441,7 @@
     </row>
     <row r="50" spans="3:13" ht="14.4">
       <c r="C50" s="49">
-        <f>$B$44-D50</f>
+        <f t="shared" si="1"/>
         <v>4.6160187655317708E-2</v>
       </c>
       <c r="D50" s="48">
@@ -8453,7 +8470,7 @@
     </row>
     <row r="51" spans="3:13" ht="14.4">
       <c r="C51" s="49">
-        <f>$B$44-D51</f>
+        <f t="shared" si="1"/>
         <v>1.7695017543862601E-2</v>
       </c>
       <c r="D51" s="48">
@@ -8481,7 +8498,7 @@
     </row>
     <row r="52" spans="3:13" ht="14.4">
       <c r="C52" s="49">
-        <f>$B$44-D52</f>
+        <f t="shared" si="1"/>
         <v>-4.4408278421804726E-3</v>
       </c>
       <c r="D52" s="47">
@@ -8509,7 +8526,7 @@
     </row>
     <row r="53" spans="3:13" ht="14.4">
       <c r="C53" s="49">
-        <f>$B$44-D53</f>
+        <f t="shared" si="1"/>
         <v>-3.1492114485889178E-2</v>
       </c>
       <c r="D53" s="47">
@@ -8671,16 +8688,16 @@
     <row r="60" spans="3:13" ht="14.4">
       <c r="E60" s="73"/>
       <c r="F60" s="72">
-        <f>F48-$E48</f>
+        <f t="shared" ref="F60:F70" si="2">F48-$E48</f>
         <v>-2.6514890372700273E-4</v>
       </c>
       <c r="G60" s="73"/>
       <c r="H60" s="72">
-        <f>H48-$E48</f>
+        <f t="shared" ref="H60:I70" si="3">H48-$E48</f>
         <v>3.2963091112836462E-5</v>
       </c>
       <c r="I60" s="72">
-        <f>I48-$E48</f>
+        <f t="shared" si="3"/>
         <v>-5.5999190372700569E-4</v>
       </c>
       <c r="M60" s="11" t="str">
@@ -8690,16 +8707,16 @@
     <row r="61" spans="3:13" ht="14.4">
       <c r="E61" s="73"/>
       <c r="F61" s="72">
-        <f>F49-$E49</f>
+        <f t="shared" si="2"/>
         <v>-2.4985567211377457E-4</v>
       </c>
       <c r="G61" s="73"/>
       <c r="H61" s="72">
-        <f>H49-$E49</f>
+        <f t="shared" si="3"/>
         <v>1.8346473636120242E-4</v>
       </c>
       <c r="I61" s="72">
-        <f>I49-$E49</f>
+        <f t="shared" si="3"/>
         <v>-6.8952367211377874E-4</v>
       </c>
       <c r="M61" s="11" t="str">
@@ -8709,16 +8726,16 @@
     <row r="62" spans="3:13" ht="14.4">
       <c r="E62" s="73"/>
       <c r="F62" s="72">
-        <f>F50-$E50</f>
+        <f t="shared" si="2"/>
         <v>-2.3233830497808305E-4</v>
       </c>
       <c r="G62" s="73"/>
       <c r="H62" s="72">
-        <f>H50-$E50</f>
+        <f t="shared" si="3"/>
         <v>2.7672188268234449E-4</v>
       </c>
       <c r="I62" s="72">
-        <f>I50-$E50</f>
+        <f t="shared" si="3"/>
         <v>-7.689673049780868E-4</v>
       </c>
       <c r="M62" s="11" t="str">
@@ -8728,16 +8745,16 @@
     <row r="63" spans="3:13" ht="14.4">
       <c r="E63" s="73"/>
       <c r="F63" s="72">
-        <f>F51-$E51</f>
+        <f t="shared" si="2"/>
         <v>-2.0549934871326447E-4</v>
       </c>
       <c r="G63" s="73"/>
       <c r="H63" s="72">
-        <f>H51-$E51</f>
+        <f t="shared" si="3"/>
         <v>3.5445282665928085E-4</v>
       </c>
       <c r="I63" s="72">
-        <f>I51-$E51</f>
+        <f t="shared" si="3"/>
         <v>-8.0755334871326911E-4</v>
       </c>
       <c r="M63" s="11" t="str">
@@ -8747,16 +8764,16 @@
     <row r="64" spans="3:13" ht="14.4">
       <c r="E64" s="73"/>
       <c r="F64" s="72">
-        <f>F52-$E52</f>
+        <f t="shared" si="2"/>
         <v>-1.8073122039533387E-4</v>
       </c>
       <c r="G64" s="73"/>
       <c r="H64" s="72">
-        <f>H52-$E52</f>
+        <f t="shared" si="3"/>
         <v>3.0689324090431985E-4</v>
       </c>
       <c r="I64" s="72">
-        <f>I52-$E52</f>
+        <f t="shared" si="3"/>
         <v>-7.0440022039533479E-4</v>
       </c>
       <c r="M64" s="11" t="str">
@@ -8766,16 +8783,16 @@
     <row r="65" spans="5:13" ht="14.4">
       <c r="E65" s="73"/>
       <c r="F65" s="72">
-        <f>F53-$E53</f>
+        <f t="shared" si="2"/>
         <v>-3.0781796069293162E-4</v>
       </c>
       <c r="G65" s="73"/>
       <c r="H65" s="72">
-        <f>H53-$E53</f>
+        <f t="shared" si="3"/>
         <v>-6.2592562598403831E-5</v>
       </c>
       <c r="I65" s="72">
-        <f>I53-$E53</f>
+        <f t="shared" si="3"/>
         <v>-5.8111931107449229E-4</v>
       </c>
       <c r="M65" s="11" t="str">
@@ -8785,16 +8802,16 @@
     <row r="66" spans="5:13" ht="14.4">
       <c r="E66" s="73"/>
       <c r="F66" s="72">
-        <f>F54-$E54</f>
+        <f t="shared" si="2"/>
         <v>-1.0257158227227649E-4</v>
       </c>
       <c r="G66" s="73"/>
       <c r="H66" s="72">
-        <f>H54-$E54</f>
+        <f t="shared" si="3"/>
         <v>-2.2131690792261908E-4</v>
       </c>
       <c r="I66" s="72">
-        <f>I54-$E54</f>
+        <f t="shared" si="3"/>
         <v>3.7690417727723885E-5</v>
       </c>
       <c r="M66" s="11" t="str">
@@ -8804,16 +8821,16 @@
     <row r="67" spans="5:13" ht="14.4">
       <c r="E67" s="73"/>
       <c r="F67" s="72">
-        <f>F55-$E55</f>
+        <f t="shared" si="2"/>
         <v>-7.1556948272093624E-5</v>
       </c>
       <c r="G67" s="73"/>
       <c r="H67" s="72">
-        <f>H55-$E55</f>
+        <f t="shared" si="3"/>
         <v>-3.2466031635390623E-4</v>
       </c>
       <c r="I67" s="72">
-        <f>I55-$E55</f>
+        <f t="shared" si="3"/>
         <v>2.3187905172790619E-4</v>
       </c>
       <c r="M67" s="11" t="str">
@@ -8823,16 +8840,16 @@
     <row r="68" spans="5:13" ht="14.4">
       <c r="E68" s="73"/>
       <c r="F68" s="72">
-        <f>F56-$E56</f>
+        <f t="shared" si="2"/>
         <v>-4.0926341106486096E-5</v>
       </c>
       <c r="G68" s="73"/>
       <c r="H68" s="72">
-        <f>H56-$E56</f>
+        <f t="shared" si="3"/>
         <v>-2.6690455214659038E-4</v>
       </c>
       <c r="I68" s="72">
-        <f>I56-$E56</f>
+        <f t="shared" si="3"/>
         <v>2.6827065889351389E-4</v>
       </c>
       <c r="M68" s="11" t="str">
@@ -8842,16 +8859,16 @@
     <row r="69" spans="5:13" ht="14.4">
       <c r="E69" s="73"/>
       <c r="F69" s="72">
-        <f>F57-$E57</f>
+        <f t="shared" si="2"/>
         <v>-2.8628011677538871E-5</v>
       </c>
       <c r="G69" s="73"/>
       <c r="H69" s="72">
-        <f>H57-$E57</f>
+        <f t="shared" si="3"/>
         <v>-1.7990501700692138E-4</v>
       </c>
       <c r="I69" s="72">
-        <f>I57-$E57</f>
+        <f t="shared" si="3"/>
         <v>2.1621588118401623E-4</v>
       </c>
       <c r="M69" s="11" t="str">
@@ -8861,16 +8878,16 @@
     <row r="70" spans="5:13" ht="14.4">
       <c r="E70" s="73"/>
       <c r="F70" s="72">
-        <f>F58-$E58</f>
+        <f t="shared" si="2"/>
         <v>-1.2551168001800049E-5</v>
       </c>
       <c r="G70" s="73"/>
       <c r="H70" s="72">
-        <f>H58-$E58</f>
+        <f t="shared" si="3"/>
         <v>-7.7004921107345681E-5</v>
       </c>
       <c r="I70" s="72">
-        <f>I58-$E58</f>
+        <f t="shared" si="3"/>
         <v>1.2904483199819994E-4</v>
       </c>
       <c r="M70" s="11" t="str">
@@ -8889,20 +8906,20 @@
     </row>
     <row r="72" spans="5:13" ht="14.4">
       <c r="E72" s="72">
-        <f>E48-MAX(($B$44-$D48),0)</f>
+        <f t="shared" ref="E72:F82" si="4">E48-MAX(($B$44-$D48),0)</f>
         <v>5.4459853877041053E-3</v>
       </c>
       <c r="F72" s="72">
-        <f>F48-MAX(($B$44-$D48),0)</f>
+        <f t="shared" si="4"/>
         <v>5.1808364839771026E-3</v>
       </c>
       <c r="G72" s="72"/>
       <c r="H72" s="72">
-        <f>H48-MAX(($B$44-$D48),0)</f>
+        <f t="shared" ref="H72:I82" si="5">H48-MAX(($B$44-$D48),0)</f>
         <v>5.4789484788169418E-3</v>
       </c>
       <c r="I72" s="72">
-        <f>I48-MAX(($B$44-$D48),0)</f>
+        <f t="shared" si="5"/>
         <v>4.8859934839770996E-3</v>
       </c>
       <c r="M72" s="11" t="str">
@@ -8911,20 +8928,20 @@
     </row>
     <row r="73" spans="5:13" ht="14.4">
       <c r="E73" s="72">
-        <f>E49-MAX(($B$44-$D49),0)</f>
+        <f t="shared" si="4"/>
         <v>9.2336396013833616E-3</v>
       </c>
       <c r="F73" s="72">
-        <f>F49-MAX(($B$44-$D49),0)</f>
+        <f t="shared" si="4"/>
         <v>8.983783929269587E-3</v>
       </c>
       <c r="G73" s="72"/>
       <c r="H73" s="72">
-        <f>H49-MAX(($B$44-$D49),0)</f>
+        <f t="shared" si="5"/>
         <v>9.417104337744564E-3</v>
       </c>
       <c r="I73" s="72">
-        <f>I49-MAX(($B$44-$D49),0)</f>
+        <f t="shared" si="5"/>
         <v>8.5441159292695829E-3</v>
       </c>
       <c r="M73" s="11" t="str">
@@ -8933,20 +8950,20 @@
     </row>
     <row r="74" spans="5:13" ht="14.4">
       <c r="E74" s="72">
-        <f>E50-MAX(($B$44-$D50),0)</f>
+        <f t="shared" si="4"/>
         <v>1.3092864649660377E-2</v>
       </c>
       <c r="F74" s="72">
-        <f>F50-MAX(($B$44-$D50),0)</f>
+        <f t="shared" si="4"/>
         <v>1.2860526344682294E-2</v>
       </c>
       <c r="G74" s="72"/>
       <c r="H74" s="72">
-        <f>H50-MAX(($B$44-$D50),0)</f>
+        <f t="shared" si="5"/>
         <v>1.3369586532342721E-2</v>
       </c>
       <c r="I74" s="72">
-        <f>I50-MAX(($B$44-$D50),0)</f>
+        <f t="shared" si="5"/>
         <v>1.232389734468229E-2</v>
       </c>
       <c r="M74" s="11" t="str">
@@ -8955,20 +8972,20 @@
     </row>
     <row r="75" spans="5:13" ht="14.4">
       <c r="E75" s="72">
-        <f>E51-MAX(($B$44-$D51),0)</f>
+        <f t="shared" si="4"/>
         <v>2.1344690804850665E-2</v>
       </c>
       <c r="F75" s="72">
-        <f>F51-MAX(($B$44-$D51),0)</f>
+        <f t="shared" si="4"/>
         <v>2.11391914561374E-2</v>
       </c>
       <c r="G75" s="72"/>
       <c r="H75" s="72">
-        <f>H51-MAX(($B$44-$D51),0)</f>
+        <f t="shared" si="5"/>
         <v>2.1699143631509946E-2</v>
       </c>
       <c r="I75" s="72">
-        <f>I51-MAX(($B$44-$D51),0)</f>
+        <f t="shared" si="5"/>
         <v>2.0537137456137396E-2</v>
       </c>
       <c r="M75" s="11" t="str">
@@ -8977,20 +8994,20 @@
     </row>
     <row r="76" spans="5:13" ht="14.4">
       <c r="E76" s="72">
-        <f>E52-MAX(($B$44-$D52),0)</f>
+        <f t="shared" si="4"/>
         <v>2.6333104220395333E-2</v>
       </c>
       <c r="F76" s="72">
-        <f>F52-MAX(($B$44-$D52),0)</f>
+        <f t="shared" si="4"/>
         <v>2.6152373E-2</v>
       </c>
       <c r="G76" s="72"/>
       <c r="H76" s="72">
-        <f>H52-MAX(($B$44-$D52),0)</f>
+        <f t="shared" si="5"/>
         <v>2.6639997461299653E-2</v>
       </c>
       <c r="I76" s="72">
-        <f>I52-MAX(($B$44-$D52),0)</f>
+        <f t="shared" si="5"/>
         <v>2.5628703999999999E-2</v>
       </c>
       <c r="M76" s="11" t="str">
@@ -8999,20 +9016,20 @@
     </row>
     <row r="77" spans="5:13" ht="14.4">
       <c r="E77" s="72">
-        <f>E53-MAX(($B$44-$D53),0)</f>
+        <f t="shared" si="4"/>
         <v>1.5151372402281888E-2</v>
       </c>
       <c r="F77" s="72">
-        <f>F53-MAX(($B$44-$D53),0)</f>
+        <f t="shared" si="4"/>
         <v>1.4843554441588956E-2</v>
       </c>
       <c r="G77" s="72"/>
       <c r="H77" s="72">
-        <f>H53-MAX(($B$44-$D53),0)</f>
+        <f t="shared" si="5"/>
         <v>1.5088779839683484E-2</v>
       </c>
       <c r="I77" s="72">
-        <f>I53-MAX(($B$44-$D53),0)</f>
+        <f t="shared" si="5"/>
         <v>1.4570253091207396E-2</v>
       </c>
       <c r="M77" s="11" t="str">
@@ -9021,20 +9038,20 @@
     </row>
     <row r="78" spans="5:13" ht="14.4">
       <c r="E78" s="72">
-        <f>E54-MAX(($B$44-$D54),0)</f>
+        <f t="shared" si="4"/>
         <v>6.2135855822722762E-3</v>
       </c>
       <c r="F78" s="72">
-        <f>F54-MAX(($B$44-$D54),0)</f>
+        <f t="shared" si="4"/>
         <v>6.1110139999999997E-3</v>
       </c>
       <c r="G78" s="72"/>
       <c r="H78" s="72">
-        <f>H54-MAX(($B$44-$D54),0)</f>
+        <f t="shared" si="5"/>
         <v>5.9922686743496571E-3</v>
       </c>
       <c r="I78" s="72">
-        <f>I54-MAX(($B$44-$D54),0)</f>
+        <f t="shared" si="5"/>
         <v>6.2512760000000001E-3</v>
       </c>
       <c r="M78" s="11" t="str">
@@ -9043,20 +9060,20 @@
     </row>
     <row r="79" spans="5:13" ht="14.4">
       <c r="E79" s="72">
-        <f>E55-MAX(($B$44-$D55),0)</f>
+        <f t="shared" si="4"/>
         <v>2.9526949482720937E-3</v>
       </c>
       <c r="F79" s="72">
-        <f>F55-MAX(($B$44-$D55),0)</f>
+        <f t="shared" si="4"/>
         <v>2.8811380000000001E-3</v>
       </c>
       <c r="G79" s="72"/>
       <c r="H79" s="72">
-        <f>H55-MAX(($B$44-$D55),0)</f>
+        <f t="shared" si="5"/>
         <v>2.6280346319181875E-3</v>
       </c>
       <c r="I79" s="72">
-        <f>I55-MAX(($B$44-$D55),0)</f>
+        <f t="shared" si="5"/>
         <v>3.1845739999999999E-3</v>
       </c>
       <c r="M79" s="11" t="str">
@@ -9065,20 +9082,20 @@
     </row>
     <row r="80" spans="5:13" ht="14.4">
       <c r="E80" s="72">
-        <f>E56-MAX(($B$44-$D56),0)</f>
+        <f t="shared" si="4"/>
         <v>1.043489341106486E-3</v>
       </c>
       <c r="F80" s="72">
-        <f>F56-MAX(($B$44-$D56),0)</f>
+        <f t="shared" si="4"/>
         <v>1.0025629999999999E-3</v>
       </c>
       <c r="G80" s="72"/>
       <c r="H80" s="72">
-        <f>H56-MAX(($B$44-$D56),0)</f>
+        <f t="shared" si="5"/>
         <v>7.7658478895989565E-4</v>
       </c>
       <c r="I80" s="72">
-        <f>I56-MAX(($B$44-$D56),0)</f>
+        <f t="shared" si="5"/>
         <v>1.3117599999999999E-3</v>
       </c>
       <c r="M80" s="11" t="str">
@@ -9087,20 +9104,20 @@
     </row>
     <row r="81" spans="5:13" ht="14.4">
       <c r="E81" s="72">
-        <f>E57-MAX(($B$44-$D57),0)</f>
+        <f t="shared" si="4"/>
         <v>4.5976211881598381E-4</v>
       </c>
       <c r="F81" s="72">
-        <f>F57-MAX(($B$44-$D57),0)</f>
+        <f t="shared" si="4"/>
         <v>4.3113410713844494E-4</v>
       </c>
       <c r="G81" s="72"/>
       <c r="H81" s="72">
-        <f>H57-MAX(($B$44-$D57),0)</f>
+        <f t="shared" si="5"/>
         <v>2.7985710180906243E-4</v>
       </c>
       <c r="I81" s="72">
-        <f>I57-MAX(($B$44-$D57),0)</f>
+        <f t="shared" si="5"/>
         <v>6.7597800000000004E-4</v>
       </c>
       <c r="M81" s="11" t="str">
@@ -9109,20 +9126,20 @@
     </row>
     <row r="82" spans="5:13" ht="14.4">
       <c r="E82" s="72">
-        <f>E58-MAX(($B$44-$D58),0)</f>
+        <f t="shared" si="4"/>
         <v>1.4112016800180006E-4</v>
       </c>
       <c r="F82" s="72">
-        <f>F58-MAX(($B$44-$D58),0)</f>
+        <f t="shared" si="4"/>
         <v>1.2856900000000001E-4</v>
       </c>
       <c r="G82" s="72"/>
       <c r="H82" s="72">
-        <f>H58-MAX(($B$44-$D58),0)</f>
+        <f t="shared" si="5"/>
         <v>6.4115246894454376E-5</v>
       </c>
       <c r="I82" s="72">
-        <f>I58-MAX(($B$44-$D58),0)</f>
+        <f t="shared" si="5"/>
         <v>2.70165E-4</v>
       </c>
       <c r="M82" s="11" t="str">
@@ -13389,19 +13406,19 @@
         <v>-2.3008375752271021E-5</v>
       </c>
       <c r="F44" s="71">
-        <f>(F40-$E40)/$E44</f>
+        <f t="shared" ref="F44:I46" si="0">(F40-$E40)/$E44</f>
         <v>-0.55558123849613061</v>
       </c>
       <c r="G44" s="71">
-        <f>(G40-$E40)/$E44</f>
+        <f t="shared" si="0"/>
         <v>-1</v>
       </c>
       <c r="H44" s="71">
-        <f>(H40-$E40)/$E44</f>
+        <f t="shared" si="0"/>
         <v>-8.8824432895024668</v>
       </c>
       <c r="I44" s="71">
-        <f>(I40-$E40)/$E44</f>
+        <f t="shared" si="0"/>
         <v>7.6316100505523758</v>
       </c>
       <c r="J44" s="69"/>
@@ -13417,19 +13434,19 @@
         <v>1.130751615962839E-7</v>
       </c>
       <c r="F45" s="71">
-        <f>(F41-$E41)/$E45</f>
+        <f t="shared" si="0"/>
         <v>-12.679726682678956</v>
       </c>
       <c r="G45" s="71">
-        <f>(G41-$E41)/$E45</f>
+        <f t="shared" si="0"/>
         <v>-1</v>
       </c>
       <c r="H45" s="71">
-        <f>(H41-$E41)/$E45</f>
+        <f t="shared" si="0"/>
         <v>429.27482727360336</v>
       </c>
       <c r="I45" s="71">
-        <f>(I41-$E41)/$E45</f>
+        <f t="shared" si="0"/>
         <v>-347.23419447154549</v>
       </c>
       <c r="J45" s="69"/>
@@ -13445,19 +13462,19 @@
         <v>-7.2917361830024743E-5</v>
       </c>
       <c r="F46" s="71">
-        <f>(F42-$E42)/$E46</f>
+        <f t="shared" si="0"/>
         <v>-0.87228065377365094</v>
       </c>
       <c r="G46" s="71">
-        <f>(G42-$E42)/$E46</f>
+        <f t="shared" si="0"/>
         <v>-1</v>
       </c>
       <c r="H46" s="71">
-        <f>(H42-$E42)/$E46</f>
+        <f t="shared" si="0"/>
         <v>-1.5589317144348065E-2</v>
       </c>
       <c r="I46" s="71">
-        <f>(I42-$E42)/$E46</f>
+        <f t="shared" si="0"/>
         <v>-1.2998631916012531</v>
       </c>
       <c r="J46" s="69"/>

</xml_diff>